<commit_message>
commit "update tipos en money"
</commit_message>
<xml_diff>
--- a/jupyter/libros/pedido.xlsx
+++ b/jupyter/libros/pedido.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcomb\Desktop\Serviya\fastapi\jupyter\libros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C68ADC-7F48-4634-AC9C-872204DE98AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A279B334-DD01-4775-BFF5-F84F023B4D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6BF431FC-B864-46C5-BAD8-9FB86F16EB2A}"/>
   </bookViews>
@@ -796,7 +796,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -812,13 +812,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -911,7 +904,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -929,9 +922,6 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1298,7 +1288,7 @@
       <c r="B2" s="5">
         <v>45395</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="4" t="s">

</xml_diff>